<commit_message>
don't save player's position
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20730" windowHeight="9172"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -85,8 +85,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -112,14 +112,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -134,7 +142,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,37 +150,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,78 +188,77 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -283,13 +283,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,13 +427,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,151 +439,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,6 +589,15 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,6 +607,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,26 +641,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,21 +671,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -695,148 +695,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1273,7 +1273,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1421,11 +1421,11 @@
       <c r="G5" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="10" t="b">
-        <v>1</v>
+      <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:9">
@@ -1450,11 +1450,11 @@
       <c r="G6" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="10" t="b">
-        <v>1</v>
+      <c r="H6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:9">

</xml_diff>

<commit_message>
dont save x,y,z to redis and mysql
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
@@ -85,9 +85,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -119,7 +119,75 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,46 +202,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,15 +241,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,7 +249,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,51 +257,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,6 +283,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -295,175 +307,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,6 +589,15 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,11 +611,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,6 +641,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -640,203 +690,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1273,7 +1273,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1418,8 +1418,8 @@
       <c r="F5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="10" t="b">
-        <v>1</v>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="H5" s="3" t="b">
         <v>0</v>
@@ -1447,8 +1447,8 @@
       <c r="F6" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="10" t="b">
-        <v>1</v>
+      <c r="G6" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="H6" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
add vector3 for Object remove x, y, z form Object
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/IObject.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
   <si>
     <t>Id</t>
   </si>
@@ -34,13 +34,7 @@
     <t>ConfigID</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
+    <t>Position</t>
   </si>
   <si>
     <t>Type</t>
@@ -52,7 +46,7 @@
     <t>int</t>
   </si>
   <si>
-    <t>float</t>
+    <t>vector3</t>
   </si>
   <si>
     <t>Public</t>
@@ -86,8 +80,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -114,20 +108,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,8 +141,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -157,37 +210,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,32 +232,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,28 +255,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -283,13 +277,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,163 +415,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,17 +635,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -676,6 +659,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -695,148 +689,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1268,22 +1262,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="2" width="10.4513274336283" customWidth="1"/>
     <col min="3" max="4" width="8.45132743362832" customWidth="1"/>
     <col min="5" max="5" width="9.45132743362832" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:9">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1305,45 +1299,33 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:7">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:9">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10" t="s">
+    <row r="3" s="2" customFormat="1" spans="1:7">
+      <c r="A3" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" spans="1:9">
-      <c r="A3" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="B3" s="9" t="b">
         <v>0</v>
@@ -1363,16 +1345,10 @@
       <c r="G3" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="10" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:9">
+    <row r="4" s="2" customFormat="1" spans="1:7">
       <c r="A4" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>1</v>
@@ -1392,104 +1368,80 @@
       <c r="G4" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="10" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:9">
+    <row r="5" s="2" customFormat="1" spans="1:7">
       <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:7">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:7">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="b">
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:9">
-      <c r="A6" s="8" t="s">
+    <row r="8" s="3" customFormat="1" spans="1:7">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:9">
-      <c r="A7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:9">
-      <c r="A8" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
       </c>
@@ -1506,31 +1458,25 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="1" ht="14.25" spans="1:6">
       <c r="A9" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F9" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 H3 I3 G4 H4 I4 G5 H5 I5 G6 H6 I6 B7:F7 G7 H7 I7 J7 B8:F8 G8 H8 I8 J8 F2:F6 F9:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4 G5 G6 B7:F7 G7 H7 B8:F8 G8 H8 F2:F6 F9:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>